<commit_message>
remade external sorting algorithms logic
</commit_message>
<xml_diff>
--- a/inputs/sorted_cities.xlsx
+++ b/inputs/sorted_cities.xlsx
@@ -61,10 +61,10 @@
     <x:t>Санкт-Петербург</x:t>
   </x:si>
   <x:si>
+    <x:t>Челябинск</x:t>
+  </x:si>
+  <x:si>
     <x:t>Уфа</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Челябинск</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -536,7 +536,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
         <x:v>5</x:v>
@@ -547,7 +547,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
         <x:v>5</x:v>

</xml_diff>